<commit_message>
updated FigureToCodeMap with Figs 16, 17
</commit_message>
<xml_diff>
--- a/FigureToCode_map.xlsx
+++ b/FigureToCode_map.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorith/Dropbox/ActiveResearch/CompMethodEvaluation/CompressionStatEvaluation/Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/compression-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE06F0D3-5E4F-2041-8F05-B6AE0E0488CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8ABB84E-6B19-B842-BA2B-8B34F0EC943F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{00C988D8-AD64-0B4D-9192-28C22C6B41AD}"/>
+    <workbookView xWindow="17900" yWindow="460" windowWidth="15700" windowHeight="20420" xr2:uid="{00C988D8-AD64-0B4D-9192-28C22C6B41AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Figure Number</t>
   </si>
@@ -49,18 +48,6 @@
     <t>./TS/Exploratory Analysis/mae_day.m</t>
   </si>
   <si>
-    <t>TSMX exploratory analysis</t>
-  </si>
-  <si>
-    <t>./TSMX/Exploratory Analysis/exploratory_analysis_tsmx.m</t>
-  </si>
-  <si>
-    <t>./TSMX/Exploratory Analysis/mae_month.m</t>
-  </si>
-  <si>
-    <t>TSMX MAE by month</t>
-  </si>
-  <si>
     <t>PRECT exploratory analysis</t>
   </si>
   <si>
@@ -73,51 +60,24 @@
     <t>./PRECT/pctRainy.m</t>
   </si>
   <si>
-    <t>./TS/Time Series/time_series_template_sz_seasonality_daily.m</t>
-  </si>
-  <si>
     <t>TS error time series (sz example)</t>
   </si>
   <si>
-    <t>TS error time series (zfp example)</t>
-  </si>
-  <si>
-    <t>./TS/Time Series/time_series_template_zfp_seasonality_daily.m</t>
-  </si>
-  <si>
     <t>TS mean errors</t>
   </si>
   <si>
     <t>./TS/Mean Errors/subaxis_template_mean.m</t>
   </si>
   <si>
-    <t>./TS/Mean Errors/sz_zoomed.m</t>
-  </si>
-  <si>
-    <t>./TS/Mean Errors/zfp_zoomed.m</t>
-  </si>
-  <si>
-    <t>./TS/Mean Errors/zfp_block_partition_justBoxLevel.m</t>
-  </si>
-  <si>
     <t>TS Z-statistics</t>
   </si>
   <si>
     <t>./TS/Z_Score/subaxis_template_zscore.m</t>
   </si>
   <si>
-    <t>TS errors (zfp tol 1e-4)</t>
-  </si>
-  <si>
-    <t>./TS/Mean Errors/zfp1e_4_TSerrors.m</t>
-  </si>
-  <si>
     <t>TS contrast variances</t>
   </si>
   <si>
-    <t>./TS/Contrast Variance/contrastVarianceEWTS_new.m</t>
-  </si>
-  <si>
     <t>TS error SDs</t>
   </si>
   <si>
@@ -130,111 +90,24 @@
     <t>./TS/Seasonality/AnnualPowerMaps_daily_new.m</t>
   </si>
   <si>
-    <t>./TS/Error Correlations/subaxis_template_corr_day_new.m</t>
-  </si>
-  <si>
     <t>TS error seasonality example</t>
   </si>
   <si>
     <t>TS error annual harmonic amplitude</t>
   </si>
   <si>
-    <t>TS error lag-1 correlations</t>
-  </si>
-  <si>
     <t>TS lag-1 correlations (deseasonalized and first differenced)</t>
   </si>
   <si>
     <t>./TS/Original Correlations/corrCoefs_TS_new.m</t>
   </si>
   <si>
-    <t>TS day with largest MAE</t>
-  </si>
-  <si>
-    <t>./TS/Min_Max MAE/spatial_plot_mae_max_day_new.m</t>
-  </si>
-  <si>
-    <t>TS day with smallest MAE</t>
-  </si>
-  <si>
-    <t>./TS/Min_Max MAE/spatial_plot_mae_min_day_new.m</t>
-  </si>
-  <si>
-    <t>TSMX error time series (sz example)</t>
-  </si>
-  <si>
-    <t>TSMX error time series (zfp example)</t>
-  </si>
-  <si>
-    <t>TSMX mean errors</t>
-  </si>
-  <si>
-    <t>./TSMX/Mean Errors/subaxis_template_mean.m</t>
-  </si>
-  <si>
-    <t>TSMX Z-statistics</t>
-  </si>
-  <si>
     <t>TS mean errors zoomed-in (sz)</t>
   </si>
   <si>
     <t>TS mean errors zoomed-in (zfp)</t>
   </si>
   <si>
-    <t>TS zfp aggregated mean errors</t>
-  </si>
-  <si>
-    <t>./TSMX/Z_Score/subaxis_template_zscore.m</t>
-  </si>
-  <si>
-    <t>TSMX contrast variances</t>
-  </si>
-  <si>
-    <t>TSMX error SDs</t>
-  </si>
-  <si>
-    <t>./TSMX/Standard Deviations/subaxis_template_sd.m</t>
-  </si>
-  <si>
-    <t>TSMX error annual harmonic amplitude</t>
-  </si>
-  <si>
-    <t>./TSMX/Contrast Variance/contrastVarianceEWTSMX.m</t>
-  </si>
-  <si>
-    <t>./TSMX/Time Series/time_series_template_sz_seasonality_month.m</t>
-  </si>
-  <si>
-    <t>./TSMX/Time Series/time_series_template_zfp_seasonality_month.m</t>
-  </si>
-  <si>
-    <t>./TSMX/Seasonality/AnnualPowerMaps_new.m</t>
-  </si>
-  <si>
-    <t>TSMX error lag-1 correlations</t>
-  </si>
-  <si>
-    <t>./TSMX/Error Correlations/subaxis_template_corr_month_new.m</t>
-  </si>
-  <si>
-    <t>TSMX lag-1 correlations (deseasonalized and first differenced)</t>
-  </si>
-  <si>
-    <t>./TSMX/Original Correlations/corrCoefs_TSMX.m</t>
-  </si>
-  <si>
-    <t>TSMX day with largest MAE</t>
-  </si>
-  <si>
-    <t>TSMX day with smallest MAE</t>
-  </si>
-  <si>
-    <t>./TSMX/Min_Max MAE/spatial_plot_mae_max_month_new.m</t>
-  </si>
-  <si>
-    <t>./TSMX/Min_Max MAE/spatial_plot_mae_min_month_new.m</t>
-  </si>
-  <si>
     <t>PRECT Example Locations</t>
   </si>
   <si>
@@ -247,10 +120,28 @@
     <t>./PRECT/dailyRainfall_oddsRain.m</t>
   </si>
   <si>
-    <t>PRECT Pr(negative rain)</t>
-  </si>
-  <si>
-    <t>./PRECT/dailyRainfall_negRain.m</t>
+    <t>./TS/Time Series/time_series_template_both_seasonality_daily.m</t>
+  </si>
+  <si>
+    <t>./TS/Mean Errors/sz_zoomed_single.m</t>
+  </si>
+  <si>
+    <t>./TS/Mean Errors/zfp_zoomed_single.m</t>
+  </si>
+  <si>
+    <t>./TS/Contrast Variance/contrastVarianceNSTS_new.m</t>
+  </si>
+  <si>
+    <t>PRECT average error</t>
+  </si>
+  <si>
+    <t>PRECT odds of rain small threshold</t>
+  </si>
+  <si>
+    <t>./PRECT/dailyRainfall_oddsRain_smallThreshold.m</t>
+  </si>
+  <si>
+    <t>./PRECT/dailyRainfall_avgError.m</t>
   </si>
 </sst>
 </file>
@@ -611,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0A698B-7460-8F48-BFF0-A6B4B752A84D}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,10 +564,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -687,7 +578,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -695,10 +586,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -706,329 +597,131 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
         <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
         <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
         <v>38</v>
-      </c>
-      <c r="C21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>